<commit_message>
Continued work on the TODO list
</commit_message>
<xml_diff>
--- a/docs/TODO.xlsx
+++ b/docs/TODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tynek\WebstormProjects\fakeStore\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\WebstormProjects\fakeStore\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98799725-DD93-4108-BAA3-F5ED9F26C254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BC168-B765-4151-BCEB-78202B353EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="13275" windowWidth="29040" windowHeight="15720" xr2:uid="{34F18800-7D7C-49F0-9E38-8C232BBC83B4}"/>
+    <workbookView xWindow="12396" yWindow="0" windowWidth="10740" windowHeight="12336" xr2:uid="{34F18800-7D7C-49F0-9E38-8C232BBC83B4}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
-  <si>
-    <t>Add a modal that notifies when registration was succesful once the user succesfully registers</t>
-  </si>
-  <si>
-    <t>// TODO: Teach myself CSS grid in order to make this layout container for the navigation and the subsequent pages. also apply media queries in order to change the layout for mobile devices.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>// TODO: Figure out how to combine media queries, viewport and conditional rendering in order to render different versions of the webpage for different devices.</t>
   </si>
@@ -87,13 +81,37 @@
   </si>
   <si>
     <t>// TODO: Implement a Home page in order to test layouts with the Layout component and develop the navigation</t>
+  </si>
+  <si>
+    <t>//TODO: Add a notification modal that informs the user of a succesful registration.</t>
+  </si>
+  <si>
+    <t>//TODO: Implement user context</t>
+  </si>
+  <si>
+    <t>//TODO: Implement cart context</t>
+  </si>
+  <si>
+    <t>//TODO: Teach myself CSS grid in order to make this layout container for the navigation and the subsequent pages. also apply media queries in order to change the layout for mobile devices.</t>
+  </si>
+  <si>
+    <t>//TODO: Implement automatic cart fetching on login and refresh</t>
+  </si>
+  <si>
+    <t>//TODO: Implement automatic logging in on refresh</t>
+  </si>
+  <si>
+    <t>//TODO: Put theme in local storage and get it on refreshes or upon loading up the page.</t>
+  </si>
+  <si>
+    <t>//TODO: Glassmorphic style / black theme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,16 +119,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,14 +149,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -133,74 +183,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -217,10 +199,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="719995"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -529,251 +511,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0C54FF-8834-4BD0-B801-E6897FE41320}">
-  <dimension ref="B2:C35"/>
+  <dimension ref="B4:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="186.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="5.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="70.5546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3">
+    <row r="12" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4">
+    </row>
+    <row r="15" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5">
+    </row>
+    <row r="16" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6">
+    </row>
+    <row r="17" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7">
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8">
+    </row>
+    <row r="19" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9">
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="3">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10">
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="3">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11">
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="3">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12">
+    </row>
+    <row r="23" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="3">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13">
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="3">
+        <v>21</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="3">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14">
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15">
+    </row>
+    <row r="29" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
+        <v>26</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>